<commit_message>
'tourney' sort key rather than 'status'...
Hmm...
</commit_message>
<xml_diff>
--- a/misc/2020-spring-honors-klask-data-exploration.xlsx
+++ b/misc/2020-spring-honors-klask-data-exploration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsteele/Documents/2020-spring-jsf-m/klask/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A286BE3-64CB-9C48-BB0A-C8C771CC265E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A057DF-1781-CE46-A4A2-07A1BC87D722}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="12340" xr2:uid="{0FB73290-3CD2-E84E-A803-A9C46CC54380}"/>
   </bookViews>
@@ -163,9 +163,6 @@
     <t>1073ed04-45ef-444e-8263-8cc77b5251e4</t>
   </si>
   <si>
-    <t>status</t>
-  </si>
-  <si>
     <t>{ 
   tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
   , tourneyName: "mita"
@@ -427,6 +424,9 @@
       }
   ]
 }</t>
+  </si>
+  <si>
+    <t>tourney</t>
   </si>
 </sst>
 </file>
@@ -993,7 +993,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1012,7 +1012,7 @@
         <v>39</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>40</v>
@@ -1023,10 +1023,10 @@
         <v>41</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -1037,7 +1037,7 @@
         <v>31</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -1048,7 +1048,7 @@
         <v>31</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -1059,7 +1059,7 @@
         <v>31</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="142" customHeight="1" x14ac:dyDescent="0.2">
@@ -1067,10 +1067,10 @@
         <v>41</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="146" customHeight="1" x14ac:dyDescent="0.2">
@@ -1078,10 +1078,10 @@
         <v>41</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="228" customHeight="1" x14ac:dyDescent="0.2">
@@ -1089,10 +1089,10 @@
         <v>41</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More compound sort keys ! ! !
I think this works ! ! !
</commit_message>
<xml_diff>
--- a/misc/2020-spring-honors-klask-data-exploration.xlsx
+++ b/misc/2020-spring-honors-klask-data-exploration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsteele/Documents/2020-spring-jsf-m/klask/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E722997A-4CAD-9A40-840F-E8134BEF6275}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53963253-7A63-F64D-A353-96EC2E6E1DD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="12340" xr2:uid="{0FB73290-3CD2-E84E-A803-A9C46CC54380}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="57">
   <si>
     <t>game</t>
   </si>
@@ -172,15 +172,139 @@
 }</t>
   </si>
   <si>
-    <t>other-attribute-columns (optional)…</t>
-  </si>
-  <si>
     <t>game:1</t>
+  </si>
+  <si>
+    <t>game:2</t>
+  </si>
+  <si>
+    <t>game:3</t>
   </si>
   <si>
     <t>{
   points: [
-        { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
+      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
+        , tourneyName: 	"mita"
+        , gameNumber:	2
+        , pointDateTime: "some datetime"
+        , scorer: "Trevor", gamePointNumber: 2
+        , scorerPointNumber: 2
+        , pointType:	"forfeit"
+        , opponent:	"Valeria" 
+      }
+      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
+        , tourneyName: 	"mita"
+        , gameNumber:	2
+        , pointDateTime: "some datetime"
+        , scorer: "Trevor", gamePointNumber: 3
+        , scorerPointNumber: 3
+        , pointType:	"forfeit"
+        , opponent:	"Valeria" 
+      }
+      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
+        , tourneyName: 	"mita"
+        , gameNumber:	2
+        , pointDateTime: "some datetime"
+        , scorer: "Trevor", gamePointNumber: 4
+        , scorerPointNumber: 4
+        , pointType:	"forfeit"
+        , opponent:	"Valeria" 
+      }
+      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
+        , tourneyName: 	"mita"
+        , gameNumber:	2
+        , pointDateTime: "some datetime"
+        , scorer: "Trevor", gamePointNumber: 5
+        , scorerPointNumber: 5
+        , pointType:	"forfeit"
+        , opponent:	"Valeria" 
+      }
+      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
+        , tourneyName: 	"mita"
+        , gameNumber:	2
+        , pointDateTime: "some datetime"
+        , scorer: "Trevor", gamePointNumber: 6
+        , scorerPointNumber: 6
+        , pointType:	"forfeit"
+        , opponent:	"Valeria" 
+      }
+  ]
+}</t>
+  </si>
+  <si>
+    <t>{
+  points: [
+      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
+        , tourneyName: 	"mita"
+        , gameNumber:	3
+        , pointDateTime: "some datetime"
+        , scorer: "Tom"
+        , gamePointNumber: 1
+        , scorerPointNumber: 1
+        , pointType:	"forfeit"
+        , opponent:	"Valeria" 
+      }
+      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
+        , tourneyName: 	"mita"
+        , gameNumber:	3
+        , pointDateTime: "some datetime"
+        , scorer: "Tom"
+        , gamePointNumber: 2
+        , scorerPointNumber: 2
+        , pointType:	"forfeit"
+        , opponent:	"Valeria" 
+      }
+      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
+        , tourneyName: 	"mita"
+        , gameNumber:	3
+        , pointDateTime: "some datetime"
+        , scorer: "Tom"
+        , gamePointNumber: 3
+        , scorerPointNumber: 3
+        , pointType:	"forfeit"
+        , opponent:	"Valeria" 
+      }
+      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
+        , tourneyName: 	"mita"
+        , gameNumber:	3
+        , pointDateTime: "some datetime"
+        , scorer: "Tom"
+        , gamePointNumber: 4
+        , scorerPointNumber: 4
+        , pointType:	"forfeit"
+        , opponent:	"Valeria" 
+      }
+      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
+        , tourneyName: 	"mita"
+        , gameNumber:	3
+        , pointDateTime: "some datetime"
+        , scorer: "Tom"
+        , gamePointNumber: 5
+        , scorerPointNumber: 5
+        , pointType:	"forfeit"
+        , opponent:	"Valeria" 
+      }
+      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
+        , tourneyName: 	"mita"
+        , gameNumber:	3
+        , pointDateTime: "some datetime"
+        , scorer: "Tom"
+        , gamePointNumber: 6
+        , scorerPointNumber: 6
+        , pointType:	"forfeit"
+        , opponent:	"Valeria"
+      }
+  ]
+}</t>
+  </si>
+  <si>
+    <t>other-attribute-columns-as-needed (optional)…</t>
+  </si>
+  <si>
+    <t>{
+  points: [
+        { 
+          tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
           , tourneyName: 	"mita"
           , gameNumber:	1
           , pointDateTime: "some datetime"
@@ -190,7 +314,8 @@
           , pointType: "score"
           , opponent: "Valeria" 
         }
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
+      , { 
+         tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
         , tourneyName: 	"mita"
         , gameNumber:	1
         , pointDateTime: "some datetime"
@@ -285,151 +410,43 @@
 }</t>
   </si>
   <si>
-    <t>game:2</t>
-  </si>
-  <si>
-    <t>game:3</t>
-  </si>
-  <si>
     <t>{
-  points: [
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	2
-        , pointDateTime: "some datetime"
-        , scorer: "Trevor", gamePointNumber: 2
-        , scorerPointNumber: 2
-        , pointType:	"forfeit"
-        , opponent:	"Valeria" 
-      }
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	2
-        , pointDateTime: "some datetime"
-        , scorer: "Trevor", gamePointNumber: 3
-        , scorerPointNumber: 3
-        , pointType:	"forfeit"
-        , opponent:	"Valeria" 
-      }
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	2
-        , pointDateTime: "some datetime"
-        , scorer: "Trevor", gamePointNumber: 4
-        , scorerPointNumber: 4
-        , pointType:	"forfeit"
-        , opponent:	"Valeria" 
-      }
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	2
-        , pointDateTime: "some datetime"
-        , scorer: "Trevor", gamePointNumber: 5
-        , scorerPointNumber: 5
-        , pointType:	"forfeit"
-        , opponent:	"Valeria" 
-      }
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	2
-        , pointDateTime: "some datetime"
-        , scorer: "Trevor", gamePointNumber: 6
-        , scorerPointNumber: 6
-        , pointType:	"forfeit"
-        , opponent:	"Valeria" 
-      }
-  ]
-}</t>
-  </si>
-  <si>
-    <t>{
-  points: [
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	3
-        , pointDateTime: "some datetime"
-        , scorer: "Tom"
-        , gamePointNumber: 1
-        , scorerPointNumber: 1
-        , pointType:	"forfeit"
-        , opponent:	"Valeria" 
-      }
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	3
-        , pointDateTime: "some datetime"
-        , scorer: "Tom"
-        , gamePointNumber: 2
-        , scorerPointNumber: 2
-        , pointType:	"forfeit"
-        , opponent:	"Valeria" 
-      }
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	3
-        , pointDateTime: "some datetime"
-        , scorer: "Tom"
-        , gamePointNumber: 3
-        , scorerPointNumber: 3
-        , pointType:	"forfeit"
-        , opponent:	"Valeria" 
-      }
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	3
-        , pointDateTime: "some datetime"
-        , scorer: "Tom"
-        , gamePointNumber: 4
-        , scorerPointNumber: 4
-        , pointType:	"forfeit"
-        , opponent:	"Valeria" 
-      }
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	3
-        , pointDateTime: "some datetime"
-        , scorer: "Tom"
-        , gamePointNumber: 5
-        , scorerPointNumber: 5
-        , pointType:	"forfeit"
-        , opponent:	"Valeria" 
-      }
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	3
-        , pointDateTime: "some datetime"
-        , scorer: "Tom"
-        , gamePointNumber: 6
-        , scorerPointNumber: 6
-        , pointType:	"forfeit"
-        , opponent:	"Valeria"
-      }
-  ]
-}</t>
-  </si>
-  <si>
-    <t>tourney</t>
-  </si>
-  <si>
-    <t>{
-  name: "Trevor"
+   tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
+  , tourneyName: 	"mita"
+  , playerName: "Tom"
   , joinedDateTime: ""
   , saltedPinForInitialing: ""
 }</t>
   </si>
   <si>
     <t>{
-  name: "Tom"
+   tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
+  , tourneyName: 	"mita"
+  , playerName: "Valeria"
   , joinedDateTime: ""
   , saltedPinForInitialing: ""
 }</t>
   </si>
   <si>
     <t>{
-  name: "Valeria"
+  tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
+  , tourneyName: 	"mita"
+  , playerName: "Trevor"
   , joinedDateTime: ""
   , saltedPinForInitialing: ""
 }</t>
+  </si>
+  <si>
+    <t>joined:Tom</t>
+  </si>
+  <si>
+    <t>joined:Valeria</t>
+  </si>
+  <si>
+    <t>joined:Trevor</t>
+  </si>
+  <si>
+    <t>tourney:20201225</t>
   </si>
 </sst>
 </file>
@@ -996,15 +1013,16 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38.83203125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="6"/>
-    <col min="3" max="3" width="32.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="41" style="6" customWidth="1"/>
+    <col min="4" max="4" width="53.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="71.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1015,7 +1033,7 @@
         <v>39</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>40</v>
@@ -1026,54 +1044,54 @@
         <v>41</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
@@ -1081,10 +1099,10 @@
         <v>41</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
@@ -1092,10 +1110,10 @@
         <v>41</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bar as sort key separator...
Colons might be found in data, E.g. times in my date time sort key section...

Saw bars on AWS video ! ! !
</commit_message>
<xml_diff>
--- a/misc/2020-spring-honors-klask-data-exploration.xlsx
+++ b/misc/2020-spring-honors-klask-data-exploration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsteele/Documents/2020-spring-jsf-m/klask/misc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thsteele\Documents\GitHub\klask\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53963253-7A63-F64D-A353-96EC2E6E1DD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096729C5-8D05-4410-8389-10A3E83AFAC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="12340" xr2:uid="{0FB73290-3CD2-E84E-A803-A9C46CC54380}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{0FB73290-3CD2-E84E-A803-A9C46CC54380}"/>
   </bookViews>
   <sheets>
     <sheet name="psami" sheetId="3" r:id="rId1"/>
@@ -172,15 +172,6 @@
 }</t>
   </si>
   <si>
-    <t>game:1</t>
-  </si>
-  <si>
-    <t>game:2</t>
-  </si>
-  <si>
-    <t>game:3</t>
-  </si>
-  <si>
     <t>{
   points: [
       , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
@@ -437,16 +428,25 @@
 }</t>
   </si>
   <si>
-    <t>joined:Tom</t>
-  </si>
-  <si>
-    <t>joined:Valeria</t>
-  </si>
-  <si>
-    <t>joined:Trevor</t>
-  </si>
-  <si>
-    <t>tourney:20201225</t>
+    <t>tourney|20201225</t>
+  </si>
+  <si>
+    <t>joined|Tom</t>
+  </si>
+  <si>
+    <t>joined|Valeria</t>
+  </si>
+  <si>
+    <t>joined|Trevor</t>
+  </si>
+  <si>
+    <t>game|1</t>
+  </si>
+  <si>
+    <t>game|2</t>
+  </si>
+  <si>
+    <t>game|3</t>
   </si>
 </sst>
 </file>
@@ -1013,19 +1013,19 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="38.83203125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="38.8125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="18.1875" style="6" customWidth="1"/>
     <col min="3" max="3" width="41" style="6" customWidth="1"/>
-    <col min="4" max="4" width="53.83203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="71.83203125" customWidth="1"/>
+    <col min="4" max="4" width="53.8125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="71.8125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
         <v>38</v>
       </c>
@@ -1033,87 +1033,87 @@
         <v>39</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="110.25" x14ac:dyDescent="0.5">
       <c r="A2" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="110.25" x14ac:dyDescent="0.5">
       <c r="A3" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="110.25" x14ac:dyDescent="0.5">
       <c r="A4" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="110.25" x14ac:dyDescent="0.5">
       <c r="A5" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="409.5" x14ac:dyDescent="0.5">
       <c r="A6" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="409.5" x14ac:dyDescent="0.5">
       <c r="A7" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="409.5" x14ac:dyDescent="0.5">
       <c r="A8" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1129,17 +1129,17 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17.6875" customWidth="1"/>
+    <col min="4" max="4" width="18.8125" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="54.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.8125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="54.8125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -1744,14 +1744,14 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="1" max="1" width="17.1875" customWidth="1"/>
+    <col min="2" max="2" width="14.1875" customWidth="1"/>
     <col min="3" max="3" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="D8" t="s">
         <v>20</v>
       </c>
@@ -1881,12 +1881,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="G9" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="G10" s="2" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
I think the final data model for game results ! ! !
</commit_message>
<xml_diff>
--- a/misc/2020-spring-honors-klask-data-exploration.xlsx
+++ b/misc/2020-spring-honors-klask-data-exploration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thsteele\Documents\GitHub\klask\misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsteele/Documents/2020-spring-jsf-m/klask/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096729C5-8D05-4410-8389-10A3E83AFAC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68BD583-81DA-1442-8854-EE7D79F532C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{0FB73290-3CD2-E84E-A803-A9C46CC54380}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="12340" xr2:uid="{0FB73290-3CD2-E84E-A803-A9C46CC54380}"/>
   </bookViews>
   <sheets>
     <sheet name="psami" sheetId="3" r:id="rId1"/>
@@ -172,233 +172,7 @@
 }</t>
   </si>
   <si>
-    <t>{
-  points: [
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	2
-        , pointDateTime: "some datetime"
-        , scorer: "Trevor", gamePointNumber: 2
-        , scorerPointNumber: 2
-        , pointType:	"forfeit"
-        , opponent:	"Valeria" 
-      }
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	2
-        , pointDateTime: "some datetime"
-        , scorer: "Trevor", gamePointNumber: 3
-        , scorerPointNumber: 3
-        , pointType:	"forfeit"
-        , opponent:	"Valeria" 
-      }
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	2
-        , pointDateTime: "some datetime"
-        , scorer: "Trevor", gamePointNumber: 4
-        , scorerPointNumber: 4
-        , pointType:	"forfeit"
-        , opponent:	"Valeria" 
-      }
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	2
-        , pointDateTime: "some datetime"
-        , scorer: "Trevor", gamePointNumber: 5
-        , scorerPointNumber: 5
-        , pointType:	"forfeit"
-        , opponent:	"Valeria" 
-      }
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	2
-        , pointDateTime: "some datetime"
-        , scorer: "Trevor", gamePointNumber: 6
-        , scorerPointNumber: 6
-        , pointType:	"forfeit"
-        , opponent:	"Valeria" 
-      }
-  ]
-}</t>
-  </si>
-  <si>
-    <t>{
-  points: [
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	3
-        , pointDateTime: "some datetime"
-        , scorer: "Tom"
-        , gamePointNumber: 1
-        , scorerPointNumber: 1
-        , pointType:	"forfeit"
-        , opponent:	"Valeria" 
-      }
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	3
-        , pointDateTime: "some datetime"
-        , scorer: "Tom"
-        , gamePointNumber: 2
-        , scorerPointNumber: 2
-        , pointType:	"forfeit"
-        , opponent:	"Valeria" 
-      }
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	3
-        , pointDateTime: "some datetime"
-        , scorer: "Tom"
-        , gamePointNumber: 3
-        , scorerPointNumber: 3
-        , pointType:	"forfeit"
-        , opponent:	"Valeria" 
-      }
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	3
-        , pointDateTime: "some datetime"
-        , scorer: "Tom"
-        , gamePointNumber: 4
-        , scorerPointNumber: 4
-        , pointType:	"forfeit"
-        , opponent:	"Valeria" 
-      }
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	3
-        , pointDateTime: "some datetime"
-        , scorer: "Tom"
-        , gamePointNumber: 5
-        , scorerPointNumber: 5
-        , pointType:	"forfeit"
-        , opponent:	"Valeria" 
-      }
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	3
-        , pointDateTime: "some datetime"
-        , scorer: "Tom"
-        , gamePointNumber: 6
-        , scorerPointNumber: 6
-        , pointType:	"forfeit"
-        , opponent:	"Valeria"
-      }
-  ]
-}</t>
-  </si>
-  <si>
     <t>other-attribute-columns-as-needed (optional)…</t>
-  </si>
-  <si>
-    <t>{
-  points: [
-        { 
-          tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-          , tourneyName: 	"mita"
-          , gameNumber:	1
-          , pointDateTime: "some datetime"
-          , scorer: "Tom"
-          , gamePointNumber: 1
-          , scorerPointNumber: 1
-          , pointType: "score"
-          , opponent: "Valeria" 
-        }
-      , { 
-         tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	1
-        , pointDateTime: "some datetime"
-        , scorer: "Valeria", gamePointNumber: 2
-        , scorerPointNumber: 1
-        , pointType:	"klask"
-        , opponent:	"Tom" }
-        , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	1
-        , pointDateTime: "some datetime"
-        , scorer: "Valeria", gamePointNumber: 3
-        , scorerPointNumber: 2
-        , pointType:	"score"
-        , opponent:	"Tom" }
-        , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	1
-        , pointDateTime: "some datetime"
-        , scorer: "Tom"
-        , gamePointNumber: 4
-        , scorerPointNumber: 2
-        , pointType: "biscuit"
-        , opponent: "Valeria" 
-      }
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	1
-        , pointDateTime: "some datetime"
-        , scorer: "Tom"
-        , gamePointNumber: 5
-        , scorerPointNumber: 3
-        , pointType: "score"
-        , opponent:	"Valeria" 
-      }
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	1
-        , pointDateTime: "some datetime"
-        , scorer: "Tom"
-        , gamePointNumber: 6
-        , scorerPointNumber: 4
-        , pointType: "score"
-        , opponent:	"Valeria" 
-      }
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	1
-        , pointDateTime: "some datetime"
-        , scorer: "Valeria", gamePointNumber: 7
-        , scorerPointNumber: 3
-        , pointType:	"biscuit"
-        , opponent:	"Tom" 
-      }
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	1
-        , pointDateTime: "some datetime"
-        , scorer: "Valeria", gamePointNumber: 8
-        , scorerPointNumber: 4
-        , pointType:	"score"
-        , opponent:	"Tom" 
-      }
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	1
-        , pointDateTime: "some datetime"
-        , scorer: "Valeria", gamePointNumber: 9
-        , scorerPointNumber: 5
-        , pointType:	"loss-control"
-        , opponent:	"Tom" 
-      }
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	1
-        , pointDateTime: "some datetime"
-        , scorer: "Valeria", gamePointNumber: 10
-        , scorerPointNumber: 6
-        , pointType:	"score"
-        , opponent:	"Tom" 
-      }
-      , { tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
-        , tourneyName: 	"mita"
-        , gameNumber:	2
-        , pointDateTime: "some datetime"
-        , scorer: "Trevor", gamePointNumber: 1
-        , scorerPointNumber: 1
-        , pointType:	"forfeit"
-        , opponent:	"Valeria" 
-      }
-  ]
-}</t>
   </si>
   <si>
     <t>{
@@ -447,6 +221,216 @@
   </si>
   <si>
     <t>game|3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      {
+          tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
+        , tourneyName: "mita"
+        , gameNumber: 1 
+        , winner: "Valeria"
+        , loser: "Tom" 
+        , points: [
+            { 
+              pointDateTime: "some datetime"
+              , scorer: "Tom"
+              , gamePointNumber: 1
+              , scorerPointNumber: 1
+              , pointType: "score"
+              , opponent: "Valeria" 
+            }
+          , { 
+              pointDateTime: "some datetime"
+              , scorer: "Valeria", gamePointNumber: 2
+              , scorerPointNumber: 1
+              , pointType:	"klask"
+              , opponent:	"Tom" 
+            }
+            , { 
+              pointDateTime: "some datetime"
+              , scorer: "Valeria", gamePointNumber: 3
+              , scorerPointNumber: 2
+              , pointType:	"score"
+              , opponent:	"Tom" 
+          }
+          , { 
+              pointDateTime: "some datetime"
+              , scorer: "Tom"
+              , gamePointNumber: 4
+              , scorerPointNumber: 2
+              , pointType: "biscuit"
+              , opponent: "Valeria" 
+          }
+          , { 
+              pointDateTime: "some datetime"
+              , scorer: "Tom"
+              , gamePointNumber: 5
+              , scorerPointNumber: 3
+              , pointType: "score"
+              , opponent:	"Valeria" 
+          }
+          , { 
+              pointDateTime: "some datetime"
+              , scorer: "Tom"
+              , gamePointNumber: 6
+              , scorerPointNumber: 4
+              , pointType: "score"
+              , opponent:	"Valeria" 
+          }
+          , { 
+              pointDateTime: "some datetime"
+              , scorer: "Valeria", gamePointNumber: 7
+              , scorerPointNumber: 3
+              , pointType:	"biscuit"
+              , opponent:	"Tom" 
+          }
+          , {
+              pointDateTime: "some datetime"
+              , scorer: "Valeria", gamePointNumber: 8
+              , scorerPointNumber: 4
+              , pointType:	"score"
+              , opponent:	"Tom" 
+          }
+          , { 
+              pointDateTime: "some datetime"
+              , scorer: "Valeria", gamePointNumber: 9
+              , scorerPointNumber: 5
+              , pointType:	"loss-control"
+              , opponent:	"Tom" 
+          }
+          , { 
+              pointDateTime: "some datetime"
+              , scorer: "Valeria", gamePointNumber: 10
+              , scorerPointNumber: 6
+              , pointType:	"score"
+              , opponent:	"Tom" 
+          }
+          , { 
+              pointDateTime: "some datetime"
+              , scorer: "Trevor", gamePointNumber: 1
+              , scorerPointNumber: 1
+              , pointType:	"forfeit"
+              , opponent:	"Valeria" 
+          }
+        ]
+      }</t>
+  </si>
+  <si>
+    <t>{
+        tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
+      , tourneyName: "mita"
+      , gameNumber: 2 
+      , winner: "Trevor"
+      , loser: "Valeria" 
+      , points: [
+          { 
+            pointDateTime: "some datetime"
+            , scorer: "Trevor"
+            , gamePointNumber: 1
+            , scorerPointNumber: 1
+            , pointType:	"forfeit"
+            , opponent:	"Valeria" 
+          }
+          , { 
+            pointDateTime: "some datetime"
+            , scorer: "Trevor"
+            , gamePointNumber: 2
+            , scorerPointNumber: 2
+            , pointType:	"forfeit"
+            , opponent:	"Valeria" 
+          }
+          , { 
+            pointDateTime: "some datetime"
+            , scorer: "Trevor"
+            , gamePointNumber: 3
+            , scorerPointNumber: 3
+            , pointType:	"forfeit"
+            , opponent:	"Valeria" 
+          }
+          , { 
+            pointDateTime: "some datetime"
+            , scorer: "Trevor"
+            , gamePointNumber: 4
+            , scorerPointNumber: 4
+            , pointType:	"forfeit"
+            , opponent:	"Valeria" 
+          }
+          , { 
+            pointDateTime: "some datetime"
+            , scorer: "Trevor"
+            , gamePointNumber: 5
+            , scorerPointNumber: 5
+            , pointType:	"forfeit"
+            , opponent:	"Valeria" 
+          }
+          , { 
+            pointDateTime: "some datetime"
+            , scorer: "Trevor"
+            , gamePointNumber: 6
+            , scorerPointNumber: 6
+            , pointType:	"forfeit"
+            , opponent:	"Valeria" 
+          }
+        ]
+      }</t>
+  </si>
+  <si>
+    <t>{
+        tourneyId: "1073ed04-45ef-444e-8263-8cc77b5251e4"
+      , tourneyName: "mita"
+      , gameNumber: 3
+      , winner: "Tom"
+      , loser: "Valeria" 
+      , points: [
+          { 
+            pointDateTime: "some datetime"
+            , scorer: "Tom"
+            , gamePointNumber: 1
+            , scorerPointNumber: 1
+            , pointType:	"forfeit"
+            , opponent:	"Valeria" 
+          }
+          , { 
+            pointDateTime: "some datetime"
+            , scorer: "Tom"
+            , gamePointNumber: 2
+            , scorerPointNumber: 2
+            , pointType:	"forfeit"
+            , opponent:	"Valeria" 
+          }
+          , { 
+            pointDateTime: "some datetime"
+            , scorer: "Tom"
+            , gamePointNumber: 3
+            , scorerPointNumber: 3
+            , pointType:	"forfeit"
+            , opponent:	"Valeria" 
+          }
+          , { 
+            pointDateTime: "some datetime"
+            , scorer: "Tom"
+            , gamePointNumber: 4
+            , scorerPointNumber: 4
+            , pointType:	"forfeit"
+            , opponent:	"Valeria" 
+          }
+          , { 
+            pointDateTime: "some datetime"
+            , scorer: "Tom"
+            , gamePointNumber: 5
+            , scorerPointNumber: 5
+            , pointType:	"forfeit"
+            , opponent:	"Valeria" 
+          }
+          , { 
+            pointDateTime: "some datetime"
+            , scorer: "Tom"
+            , gamePointNumber: 6
+            , scorerPointNumber: 6
+            , pointType:	"forfeit"
+            , opponent:	"Valeria" 
+          }
+        ]
+      }</t>
   </si>
 </sst>
 </file>
@@ -1012,20 +996,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{403B472A-466F-184F-B08D-048A36C02FB5}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.8125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="18.1875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="38.83203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="6" customWidth="1"/>
     <col min="3" max="3" width="41" style="6" customWidth="1"/>
-    <col min="4" max="4" width="53.8125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="71.8125" customWidth="1"/>
+    <col min="4" max="4" width="53.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="71.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>38</v>
       </c>
@@ -1033,87 +1017,87 @@
         <v>39</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="110.25" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="110.25" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="110.25" x14ac:dyDescent="0.5">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="110.25" x14ac:dyDescent="0.5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="409.5" x14ac:dyDescent="0.5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="409.5" x14ac:dyDescent="0.5">
+    </row>
+    <row r="7" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="409.5" x14ac:dyDescent="0.5">
+    </row>
+    <row r="8" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1129,17 +1113,17 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="2" max="2" width="17.6875" customWidth="1"/>
-    <col min="4" max="4" width="18.8125" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="12.8125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="54.8125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="54.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1165,7 +1149,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1191,7 +1175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1220,7 +1204,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1246,7 +1230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1275,7 +1259,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1301,7 +1285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1327,7 +1311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1353,7 +1337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1379,7 +1363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1405,7 +1389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1431,7 +1415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1454,7 +1438,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1477,7 +1461,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1503,7 +1487,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1526,7 +1510,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1549,7 +1533,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1575,7 +1559,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -1598,7 +1582,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -1624,7 +1608,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -1647,7 +1631,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1670,7 +1654,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1693,7 +1677,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1716,7 +1700,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -1744,14 +1728,14 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.1875" customWidth="1"/>
-    <col min="2" max="2" width="14.1875" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
     <col min="3" max="3" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1768,7 +1752,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1785,7 +1769,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1802,7 +1786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1819,7 +1803,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1836,7 +1820,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1856,7 +1840,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1873,7 +1857,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
         <v>20</v>
       </c>
@@ -1881,12 +1865,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G9" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G10" s="2" t="s">
         <v>34</v>
       </c>

</xml_diff>